<commit_message>
Added passport priority notes handler to hca.py
</commit_message>
<xml_diff>
--- a/resources/hca_master_fake.xlsx
+++ b/resources/hca_master_fake.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otrob\Documents\Dev\HaitiApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE17B2B9-DD8A-4C2B-9AC8-F6D68C144C34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238A324D-FE93-4CA9-83EB-7AC0E9339ACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="406" xr2:uid="{79D572EB-08E4-486B-8004-00E6DEB842A1}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16945" uniqueCount="4055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16930" uniqueCount="4055">
   <si>
     <t>id</t>
   </si>
@@ -12819,7 +12819,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC57" sqref="AC57"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>